<commit_message>
update comparison results for variable efficiency
</commit_message>
<xml_diff>
--- a/spine_projects/02_output_data/comparison_piecewise_operating.xlsx
+++ b/spine_projects/02_output_data/comparison_piecewise_operating.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\02_output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D176BA9-742E-468E-AD5C-97CCB859816E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE996FBF-59EE-45FC-9D08-1628F1FAFDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{92573A4F-CF48-4568-895A-C6D4F40C52D8}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{92573A4F-CF48-4568-895A-C6D4F40C52D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="on Input relation" sheetId="1" r:id="rId1"/>
+    <sheet name="on Output relation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Power Input</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Identical</t>
   </si>
 </sst>
 </file>
@@ -441,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B09DF4-4240-4045-87D1-2B73DB7753A8}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
@@ -1260,4 +1267,1056 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6C61C9-01A5-47E6-8D08-E69E18673784}">
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>13.3</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <f>B2/A2</f>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E2">
+        <f>IF($B2&gt;$N$2,$N$2*$P$2,B2*$O$2)</f>
+        <v>13.3</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" ref="F2">IF(($B2-$N$2)&gt;(0),_xlfn.IFS(B2&gt;($N$2+$N$3),$N$3*$P$3,($B2-$N$2)&gt;(0),(B2-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>IF(($B2-($N$2+$N$3))&gt;(0),(B2-($N$2+$N$3))*$P$4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(E2:G2)</f>
+        <v>13.3</v>
+      </c>
+      <c r="I2">
+        <f>H2/B2</f>
+        <v>1.33</v>
+      </c>
+      <c r="J2">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K2" t="b">
+        <f>EXACT(J2,I2)</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0.4</v>
+      </c>
+      <c r="N2">
+        <v>15.037593984962406</v>
+      </c>
+      <c r="O2">
+        <v>1.33</v>
+      </c>
+      <c r="P2">
+        <f>O2</f>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>27.24812</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C25" si="0">B3/A3</f>
+        <v>0.73399559309045903</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E25" si="1">IF($B3&gt;$N$2,$N$2*$P$2,B3*$O$2)</f>
+        <v>20</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3">IF(($B3-$N$2)&gt;(0),_xlfn.IFS(B3&gt;($N$2+$N$3),$N$3*$P$3,($B3-$N$2)&gt;(0),(B3-$N$2)*$P$3),0)</f>
+        <v>7.1458646616541346</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G25" si="2">IF(($B3-($N$2+$N$3))&gt;(0),(B3-($N$2+$N$3))*$P$4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H25" si="3">SUM(E3:G3)</f>
+        <v>27.145864661654134</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="4">H3/B3</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="J3">
+        <f>($N$2*$O$2+(B3-$N$2)*$O$3)/B3</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="K3" t="b">
+        <f t="shared" ref="K3:K25" si="5">EXACT(J3,I3)</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.7</v>
+      </c>
+      <c r="N3">
+        <v>10.48951048951049</v>
+      </c>
+      <c r="O3">
+        <v>1.44</v>
+      </c>
+      <c r="P3">
+        <f>O3</f>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>34.479219999999998</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.72507440713566029</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">IF(($B4-$N$2)&gt;(0),_xlfn.IFS(B4&gt;($N$2+$N$3),$N$3*$P$3,($B4-$N$2)&gt;(0),(B4-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J4">
+        <f>($N$2*$O$2+(B4-$N$2)*$O$3)/B4</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>9.7402597402597397</v>
+      </c>
+      <c r="O4">
+        <v>1.54</v>
+      </c>
+      <c r="P4">
+        <f>O4</f>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6.65</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>6.65</v>
+      </c>
+      <c r="F5" cm="1">
+        <f t="array" ref="F5">IF(($B5-$N$2)&gt;(0),_xlfn.IFS(B5&gt;($N$2+$N$3),$N$3*$P$3,($B5-$N$2)&gt;(0),(B5-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>6.65</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J5">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K5" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>13.3</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="F6" cm="1">
+        <f t="array" ref="F6">IF(($B6-$N$2)&gt;(0),_xlfn.IFS(B6&gt;($N$2+$N$3),$N$3*$P$3,($B6-$N$2)&gt;(0),(B6-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J6">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K6" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>20.048120000000001</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.74819983120611799</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>19.950000000000003</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" ref="F7">IF(($B7-$N$2)&gt;(0),_xlfn.IFS(B7&gt;($N$2+$N$3),$N$3*$P$3,($B7-$N$2)&gt;(0),(B7-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>19.950000000000003</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>1.3300000000000003</v>
+      </c>
+      <c r="J7">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K7" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>27.24812</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.73399559309045903</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" ref="F8">IF(($B8-$N$2)&gt;(0),_xlfn.IFS(B8&gt;($N$2+$N$3),$N$3*$P$3,($B8-$N$2)&gt;(0),(B8-$N$2)*$P$3),0)</f>
+        <v>7.1458646616541346</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>27.145864661654134</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="J8">
+        <f>($N$2*$O$2+(B8-$N$2)*$O$3)/B8</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="K8" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>42.179220000000001</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.71125070591632555</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F9" cm="1">
+        <f t="array" ref="F9">IF(($B9-$N$2)&gt;(0),_xlfn.IFS(B9&gt;($N$2+$N$3),$N$3*$P$3,($B9-$N$2)&gt;(0),(B9-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>6.8882591093117398</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>41.993154214206847</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="J9">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B9-$N$2-$N$3)*$O$4)/B9</f>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="K9" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>49.879219999999997</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.70169501447697058</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F10" cm="1">
+        <f t="array" ref="F10">IF(($B10-$N$2)&gt;(0),_xlfn.IFS(B10&gt;($N$2+$N$3),$N$3*$P$3,($B10-$N$2)&gt;(0),(B10-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>14.588259109311741</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>49.693154214206849</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>1.4198044061201958</v>
+      </c>
+      <c r="J10">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B10-$N$2-$N$3)*$O$4)/B10</f>
+        <v>1.4198044061201958</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>45.259219999999999</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.70703825651436325</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F11" cm="1">
+        <f t="array" ref="F11">IF(($B11-$N$2)&gt;(0),_xlfn.IFS(B11&gt;($N$2+$N$3),$N$3*$P$3,($B11-$N$2)&gt;(0),(B11-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>9.9682591093117399</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>45.073154214206845</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>1.4085360691939639</v>
+      </c>
+      <c r="J11">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B11-$N$2-$N$3)*$O$4)/B11</f>
+        <v>1.4085360691939639</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>36.019219999999997</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.72183684155292649</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F12" cm="1">
+        <f t="array" ref="F12">IF(($B12-$N$2)&gt;(0),_xlfn.IFS(B12&gt;($N$2+$N$3),$N$3*$P$3,($B12-$N$2)&gt;(0),(B12-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0.72825910931173998</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>35.83315421420685</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>1.3781982390079557</v>
+      </c>
+      <c r="J12">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B12-$N$2-$N$3)*$O$4)/B12</f>
+        <v>1.3781982390079557</v>
+      </c>
+      <c r="K12" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>33.008119999999998</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.72709381812717599</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F13" cm="1">
+        <f t="array" ref="F13">IF(($B13-$N$2)&gt;(0),_xlfn.IFS(B13&gt;($N$2+$N$3),$N$3*$P$3,($B13-$N$2)&gt;(0),(B13-$N$2)*$P$3),0)</f>
+        <v>12.905864661654135</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>32.905864661654135</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>1.3710776942355889</v>
+      </c>
+      <c r="J13">
+        <f>($N$2*$O$2+(B13-$N$2)*$O$3)/B13</f>
+        <v>1.3710776942355889</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>24.368120000000001</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.7386700328133643</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F14" cm="1">
+        <f t="array" ref="F14">IF(($B14-$N$2)&gt;(0),_xlfn.IFS(B14&gt;($N$2+$N$3),$N$3*$P$3,($B14-$N$2)&gt;(0),(B14-$N$2)*$P$3),0)</f>
+        <v>4.2658646616541347</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>24.265864661654135</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="J14">
+        <f>($N$2*$O$2+(B14-$N$2)*$O$3)/B14</f>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>5.32</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>5.32</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" ref="F15">IF(($B15-$N$2)&gt;(0),_xlfn.IFS(B15&gt;($N$2+$N$3),$N$3*$P$3,($B15-$N$2)&gt;(0),(B15-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>5.32</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J15">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K15" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>13.3</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="F16" cm="1">
+        <f t="array" ref="F16">IF(($B16-$N$2)&gt;(0),_xlfn.IFS(B16&gt;($N$2+$N$3),$N$3*$P$3,($B16-$N$2)&gt;(0),(B16-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J16">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K16" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>34.479219999999998</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.72507440713566029</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F17" cm="1">
+        <f t="array" ref="F17">IF(($B17-$N$2)&gt;(0),_xlfn.IFS(B17&gt;($N$2+$N$3),$N$3*$P$3,($B17-$N$2)&gt;(0),(B17-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J17">
+        <f>($N$2*$O$2+(B17-$N$2)*$O$3)/B17</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K17" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>34.479219999999998</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.72507440713566029</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F18" cm="1">
+        <f t="array" ref="F18">IF(($B18-$N$2)&gt;(0),_xlfn.IFS(B18&gt;($N$2+$N$3),$N$3*$P$3,($B18-$N$2)&gt;(0),(B18-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J18">
+        <f>($N$2*$O$2+(B18-$N$2)*$O$3)/B18</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K18" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>42.179220000000001</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.71125070591632555</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F19" cm="1">
+        <f t="array" ref="F19">IF(($B19-$N$2)&gt;(0),_xlfn.IFS(B19&gt;($N$2+$N$3),$N$3*$P$3,($B19-$N$2)&gt;(0),(B19-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>6.8882591093117398</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>41.993154214206847</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="J19">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B19-$N$2-$N$3)*$O$4)/B19</f>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="K19" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>27.24812</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.73399559309045903</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F20" cm="1">
+        <f t="array" ref="F20">IF(($B20-$N$2)&gt;(0),_xlfn.IFS(B20&gt;($N$2+$N$3),$N$3*$P$3,($B20-$N$2)&gt;(0),(B20-$N$2)*$P$3),0)</f>
+        <v>7.1458646616541346</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>27.145864661654134</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="J20">
+        <f>($N$2*$O$2+(B20-$N$2)*$O$3)/B20</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="K20" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>13.3</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="F21" cm="1">
+        <f t="array" ref="F21">IF(($B21-$N$2)&gt;(0),_xlfn.IFS(B21&gt;($N$2+$N$3),$N$3*$P$3,($B21-$N$2)&gt;(0),(B21-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J21">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K21" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>6.65</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>6.65</v>
+      </c>
+      <c r="F22" cm="1">
+        <f t="array" ref="F22">IF(($B22-$N$2)&gt;(0),_xlfn.IFS(B22&gt;($N$2+$N$3),$N$3*$P$3,($B22-$N$2)&gt;(0),(B22-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>6.65</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J22">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K22" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>42.179220000000001</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.71125070591632555</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F23" cm="1">
+        <f t="array" ref="F23">IF(($B23-$N$2)&gt;(0),_xlfn.IFS(B23&gt;($N$2+$N$3),$N$3*$P$3,($B23-$N$2)&gt;(0),(B23-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>6.8882591093117398</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>41.993154214206847</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="J23">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B23-$N$2-$N$3)*$O$4)/B23</f>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="K23" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>34.479219999999998</v>
+      </c>
+      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.72507440713566029</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F24" cm="1">
+        <f t="array" ref="F24">IF(($B24-$N$2)&gt;(0),_xlfn.IFS(B24&gt;($N$2+$N$3),$N$3*$P$3,($B24-$N$2)&gt;(0),(B24-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J24">
+        <f>($N$2*$O$2+(B24-$N$2)*$O$3)/B24</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K24" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24.368120000000001</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.7386700328133643</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F25" cm="1">
+        <f t="array" ref="F25">IF(($B25-$N$2)&gt;(0),_xlfn.IFS(B25&gt;($N$2+$N$3),$N$3*$P$3,($B25-$N$2)&gt;(0),(B25-$N$2)*$P$3),0)</f>
+        <v>4.2658646616541347</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>24.265864661654135</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="J25">
+        <f>($N$2*$O$2+(B25-$N$2)*$O$3)/B25</f>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="K25" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update comparison of var eff approach
</commit_message>
<xml_diff>
--- a/spine_projects/02_output_data/comparison_piecewise_operating.xlsx
+++ b/spine_projects/02_output_data/comparison_piecewise_operating.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\02_output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE996FBF-59EE-45FC-9D08-1628F1FAFDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A5B65-6673-4EC8-92FF-2467356BBEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{92573A4F-CF48-4568-895A-C6D4F40C52D8}"/>
   </bookViews>
   <sheets>
     <sheet name="on Input relation" sheetId="1" r:id="rId1"/>
     <sheet name="on Output relation" sheetId="2" r:id="rId2"/>
+    <sheet name="in_and_dec_eff" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="12">
   <si>
     <t>Power Input</t>
   </si>
@@ -1271,10 +1272,1214 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6C61C9-01A5-47E6-8D08-E69E18673784}">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="T1">
+        <v>14.388489208599999</v>
+      </c>
+      <c r="V1">
+        <f>T1*0.65</f>
+        <v>9.3525179855899996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <f>B2/A2</f>
+        <v>0.75000000000187494</v>
+      </c>
+      <c r="E2">
+        <f>IF($B2&gt;$N$2,$N$2*$P$2,B2*$O$2)</f>
+        <v>13.3</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" ref="F2">IF(($B2-$N$2)&gt;(0),_xlfn.IFS(B2&gt;($N$2+$N$3),$N$3*$P$3,($B2-$N$2)&gt;(0),(B2-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>IF(($B2-($N$2+$N$3))&gt;(0),(B2-($N$2+$N$3))*$P$4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(E2:G2)</f>
+        <v>13.3</v>
+      </c>
+      <c r="I2">
+        <f>H2/B2</f>
+        <v>1.33</v>
+      </c>
+      <c r="J2">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K2" t="b">
+        <f>EXACT(J2,I2)</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0.4</v>
+      </c>
+      <c r="N2">
+        <v>15.037593984962406</v>
+      </c>
+      <c r="O2">
+        <v>1.33</v>
+      </c>
+      <c r="P2">
+        <f>O2</f>
+        <v>1.33</v>
+      </c>
+      <c r="S2">
+        <v>27.5</v>
+      </c>
+      <c r="T2">
+        <v>28.776978417300001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>27.5</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C25" si="0">B3/A3</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E25" si="1">IF($B3&gt;$N$2,$N$2*$P$2,B3*$O$2)</f>
+        <v>20</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3">IF(($B3-$N$2)&gt;(0),_xlfn.IFS(B3&gt;($N$2+$N$3),$N$3*$P$3,($B3-$N$2)&gt;(0),(B3-$N$2)*$P$3),0)</f>
+        <v>7.1458646616541346</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G25" si="2">IF(($B3-($N$2+$N$3))&gt;(0),(B3-($N$2+$N$3))*$P$4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H25" si="3">SUM(E3:G3)</f>
+        <v>27.145864661654134</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="4">H3/B3</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="J3">
+        <f>($N$2*$O$2+(B3-$N$2)*$O$3)/B3</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="K3" t="b">
+        <f t="shared" ref="K3:K25" si="5">EXACT(J3,I3)</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.7</v>
+      </c>
+      <c r="N3">
+        <v>10.48951048951049</v>
+      </c>
+      <c r="O3">
+        <v>1.44</v>
+      </c>
+      <c r="P3">
+        <f>O3</f>
+        <v>1.44</v>
+      </c>
+      <c r="S3">
+        <v>35</v>
+      </c>
+      <c r="T3">
+        <v>35.971223021599997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">IF(($B4-$N$2)&gt;(0),_xlfn.IFS(B4&gt;($N$2+$N$3),$N$3*$P$3,($B4-$N$2)&gt;(0),(B4-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J4">
+        <f>($N$2*$O$2+(B4-$N$2)*$O$3)/B4</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>9.7402597402597397</v>
+      </c>
+      <c r="O4">
+        <v>1.54</v>
+      </c>
+      <c r="P4">
+        <f>O4</f>
+        <v>1.54</v>
+      </c>
+      <c r="S4">
+        <v>6.6666666666700003</v>
+      </c>
+      <c r="T4">
+        <v>7.1942446043199997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6.6666666666700003</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.74999999999962497</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>6.65</v>
+      </c>
+      <c r="F5" cm="1">
+        <f t="array" ref="F5">IF(($B5-$N$2)&gt;(0),_xlfn.IFS(B5&gt;($N$2+$N$3),$N$3*$P$3,($B5-$N$2)&gt;(0),(B5-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>6.65</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J5">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K5" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="T5">
+        <v>14.388489208599999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.75000000000187494</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="F6" cm="1">
+        <f t="array" ref="F6">IF(($B6-$N$2)&gt;(0),_xlfn.IFS(B6&gt;($N$2+$N$3),$N$3*$P$3,($B6-$N$2)&gt;(0),(B6-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J6">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K6" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>20.357142857100001</v>
+      </c>
+      <c r="T6">
+        <v>21.582733812899999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>20.357142857100001</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.73684210526470906</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>19.950000000000003</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" ref="F7">IF(($B7-$N$2)&gt;(0),_xlfn.IFS(B7&gt;($N$2+$N$3),$N$3*$P$3,($B7-$N$2)&gt;(0),(B7-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>19.950000000000003</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>1.3300000000000003</v>
+      </c>
+      <c r="J7">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K7" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>27.5</v>
+      </c>
+      <c r="T7">
+        <v>28.776978417300001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>27.5</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" ref="F8">IF(($B8-$N$2)&gt;(0),_xlfn.IFS(B8&gt;($N$2+$N$3),$N$3*$P$3,($B8-$N$2)&gt;(0),(B8-$N$2)*$P$3),0)</f>
+        <v>7.1458646616541346</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>27.145864661654134</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="J8">
+        <f>($N$2*$O$2+(B8-$N$2)*$O$3)/B8</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="K8" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>42.692307692299998</v>
+      </c>
+      <c r="T8">
+        <v>43.1654676259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>42.692307692299998</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.70270270270282931</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F9" cm="1">
+        <f t="array" ref="F9">IF(($B9-$N$2)&gt;(0),_xlfn.IFS(B9&gt;($N$2+$N$3),$N$3*$P$3,($B9-$N$2)&gt;(0),(B9-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>6.8882591093117398</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>41.993154214206847</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="J9">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B9-$N$2-$N$3)*$O$4)/B9</f>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="K9" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>50</v>
+      </c>
+      <c r="T9">
+        <v>50</v>
+      </c>
+      <c r="V9">
+        <f>20*0.65+15*0.7+15*0.75</f>
+        <v>34.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F10" cm="1">
+        <f t="array" ref="F10">IF(($B10-$N$2)&gt;(0),_xlfn.IFS(B10&gt;($N$2+$N$3),$N$3*$P$3,($B10-$N$2)&gt;(0),(B10-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>14.588259109311741</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>49.693154214206849</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>1.4198044061201958</v>
+      </c>
+      <c r="J10">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B10-$N$2-$N$3)*$O$4)/B10</f>
+        <v>1.4198044061201958</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>45.7692307692</v>
+      </c>
+      <c r="T10">
+        <v>46.043165467599998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>45.7692307692</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.69915966386601625</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F11" cm="1">
+        <f t="array" ref="F11">IF(($B11-$N$2)&gt;(0),_xlfn.IFS(B11&gt;($N$2+$N$3),$N$3*$P$3,($B11-$N$2)&gt;(0),(B11-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>9.9682591093117399</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>45.073154214206845</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>1.4085360691939639</v>
+      </c>
+      <c r="J11">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B11-$N$2-$N$3)*$O$4)/B11</f>
+        <v>1.4085360691939639</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>36.538461538500002</v>
+      </c>
+      <c r="T11">
+        <v>37.410071942400002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>36.538461538500002</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.71157894736767202</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F12" cm="1">
+        <f t="array" ref="F12">IF(($B12-$N$2)&gt;(0),_xlfn.IFS(B12&gt;($N$2+$N$3),$N$3*$P$3,($B12-$N$2)&gt;(0),(B12-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0.72825910931173998</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>35.83315421420685</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>1.3781982390079557</v>
+      </c>
+      <c r="J12">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B12-$N$2-$N$3)*$O$4)/B12</f>
+        <v>1.3781982390079557</v>
+      </c>
+      <c r="K12" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>33.461538461499998</v>
+      </c>
+      <c r="T12">
+        <v>34.532374100699997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>33.461538461499998</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.71724137931116927</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F13" cm="1">
+        <f t="array" ref="F13">IF(($B13-$N$2)&gt;(0),_xlfn.IFS(B13&gt;($N$2+$N$3),$N$3*$P$3,($B13-$N$2)&gt;(0),(B13-$N$2)*$P$3),0)</f>
+        <v>12.905864661654135</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>32.905864661654135</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>1.3710776942355889</v>
+      </c>
+      <c r="J13">
+        <f>($N$2*$O$2+(B13-$N$2)*$O$3)/B13</f>
+        <v>1.3710776942355889</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>24.642857142899999</v>
+      </c>
+      <c r="T13">
+        <v>25.899280575500001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>24.642857142899999</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.73043478260742534</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F14" cm="1">
+        <f t="array" ref="F14">IF(($B14-$N$2)&gt;(0),_xlfn.IFS(B14&gt;($N$2+$N$3),$N$3*$P$3,($B14-$N$2)&gt;(0),(B14-$N$2)*$P$3),0)</f>
+        <v>4.2658646616541347</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>24.265864661654135</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="J14">
+        <f>($N$2*$O$2+(B14-$N$2)*$O$3)/B14</f>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>5.3333333333299997</v>
+      </c>
+      <c r="T14">
+        <v>5.7553956834499997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>5.3333333333299997</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.75000000000046874</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>5.32</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" ref="F15">IF(($B15-$N$2)&gt;(0),_xlfn.IFS(B15&gt;($N$2+$N$3),$N$3*$P$3,($B15-$N$2)&gt;(0),(B15-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>5.32</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J15">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K15" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="T15">
+        <v>14.388489208599999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.75000000000187494</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="F16" cm="1">
+        <f t="array" ref="F16">IF(($B16-$N$2)&gt;(0),_xlfn.IFS(B16&gt;($N$2+$N$3),$N$3*$P$3,($B16-$N$2)&gt;(0),(B16-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J16">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K16" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>35</v>
+      </c>
+      <c r="T16">
+        <v>35.971223021599997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F17" cm="1">
+        <f t="array" ref="F17">IF(($B17-$N$2)&gt;(0),_xlfn.IFS(B17&gt;($N$2+$N$3),$N$3*$P$3,($B17-$N$2)&gt;(0),(B17-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J17">
+        <f>($N$2*$O$2+(B17-$N$2)*$O$3)/B17</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K17" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>35</v>
+      </c>
+      <c r="T17">
+        <v>35.971223021599997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F18" cm="1">
+        <f t="array" ref="F18">IF(($B18-$N$2)&gt;(0),_xlfn.IFS(B18&gt;($N$2+$N$3),$N$3*$P$3,($B18-$N$2)&gt;(0),(B18-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J18">
+        <f>($N$2*$O$2+(B18-$N$2)*$O$3)/B18</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K18" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>42.692307692299998</v>
+      </c>
+      <c r="T18">
+        <v>43.1654676259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>42.692307692299998</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.70270270270282931</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F19" cm="1">
+        <f t="array" ref="F19">IF(($B19-$N$2)&gt;(0),_xlfn.IFS(B19&gt;($N$2+$N$3),$N$3*$P$3,($B19-$N$2)&gt;(0),(B19-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>6.8882591093117398</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>41.993154214206847</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="J19">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B19-$N$2-$N$3)*$O$4)/B19</f>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="K19" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>27.5</v>
+      </c>
+      <c r="T19">
+        <v>28.776978417300001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>27.5</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F20" cm="1">
+        <f t="array" ref="F20">IF(($B20-$N$2)&gt;(0),_xlfn.IFS(B20&gt;($N$2+$N$3),$N$3*$P$3,($B20-$N$2)&gt;(0),(B20-$N$2)*$P$3),0)</f>
+        <v>7.1458646616541346</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>27.145864661654134</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="J20">
+        <f>($N$2*$O$2+(B20-$N$2)*$O$3)/B20</f>
+        <v>1.3572932330827068</v>
+      </c>
+      <c r="K20" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="T20">
+        <v>14.388489208599999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>13.333333333300001</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.75000000000187494</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="F21" cm="1">
+        <f t="array" ref="F21">IF(($B21-$N$2)&gt;(0),_xlfn.IFS(B21&gt;($N$2+$N$3),$N$3*$P$3,($B21-$N$2)&gt;(0),(B21-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J21">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K21" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>6.6666666666700003</v>
+      </c>
+      <c r="T21">
+        <v>7.1942446043199997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>6.6666666666700003</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.74999999999962497</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>6.65</v>
+      </c>
+      <c r="F22" cm="1">
+        <f t="array" ref="F22">IF(($B22-$N$2)&gt;(0),_xlfn.IFS(B22&gt;($N$2+$N$3),$N$3*$P$3,($B22-$N$2)&gt;(0),(B22-$N$2)*$P$3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>6.65</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="J22">
+        <f>1*$O$2</f>
+        <v>1.33</v>
+      </c>
+      <c r="K22" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>42.692307692299998</v>
+      </c>
+      <c r="T22">
+        <v>43.1654676259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>42.692307692299998</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.70270270270282931</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F23" cm="1">
+        <f t="array" ref="F23">IF(($B23-$N$2)&gt;(0),_xlfn.IFS(B23&gt;($N$2+$N$3),$N$3*$P$3,($B23-$N$2)&gt;(0),(B23-$N$2)*$P$3),0)</f>
+        <v>15.104895104895105</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>6.8882591093117398</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>41.993154214206847</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="J23">
+        <f>($N$2*$O$2+($N$3)*$O$3+(B23-$N$2-$N$3)*$O$4)/B23</f>
+        <v>1.3997718071402283</v>
+      </c>
+      <c r="K23" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>35</v>
+      </c>
+      <c r="T23">
+        <v>35.971223021599997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F24" cm="1">
+        <f t="array" ref="F24">IF(($B24-$N$2)&gt;(0),_xlfn.IFS(B24&gt;($N$2+$N$3),$N$3*$P$3,($B24-$N$2)&gt;(0),(B24-$N$2)*$P$3),0)</f>
+        <v>14.345864661654135</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>34.345864661654133</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="J24">
+        <f>($N$2*$O$2+(B24-$N$2)*$O$3)/B24</f>
+        <v>1.3738345864661654</v>
+      </c>
+      <c r="K24" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>24.642857142899999</v>
+      </c>
+      <c r="T24">
+        <v>25.899280575500001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24.642857142899999</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.73043478260742534</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F25" cm="1">
+        <f t="array" ref="F25">IF(($B25-$N$2)&gt;(0),_xlfn.IFS(B25&gt;($N$2+$N$3),$N$3*$P$3,($B25-$N$2)&gt;(0),(B25-$N$2)*$P$3),0)</f>
+        <v>4.2658646616541347</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>24.265864661654135</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="J25">
+        <f>($N$2*$O$2+(B25-$N$2)*$O$3)/B25</f>
+        <v>1.3481035923141187</v>
+      </c>
+      <c r="K25" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04D8C59-FBAE-46EC-91CE-2E203BD2B0EB}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1319,14 +2524,14 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>13.3</v>
+        <v>13.468013468000001</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
         <f>B2/A2</f>
-        <v>0.75187969924812026</v>
+        <v>0.74250000000074245</v>
       </c>
       <c r="E2">
         <f>IF($B2&gt;$N$2,$N$2*$P$2,B2*$O$2)</f>
@@ -1372,14 +2577,14 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>27.24812</v>
+        <v>27.357142857100001</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C25" si="0">B3/A3</f>
-        <v>0.73399559309045903</v>
+        <v>0.73107049608469621</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E25" si="1">IF($B3&gt;$N$2,$N$2*$P$2,B3*$O$2)</f>
@@ -1425,14 +2630,14 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>34.479219999999998</v>
+        <v>34.5</v>
       </c>
       <c r="B4">
         <v>25</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.72507440713566029</v>
+        <v>0.72463768115942029</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
@@ -1478,14 +2683,14 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>6.65</v>
+        <v>6.7340067340100003</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.75187969924812026</v>
+        <v>0.74249999999963989</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
@@ -1518,14 +2723,14 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>13.3</v>
+        <v>13.468013468000001</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.75187969924812026</v>
+        <v>0.74250000000074245</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
@@ -1558,14 +2763,14 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>20.048120000000001</v>
+        <v>20.214285714300001</v>
       </c>
       <c r="B7">
         <v>15</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.74819983120611799</v>
+        <v>0.7420494699641399</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
@@ -1598,14 +2803,14 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>27.24812</v>
+        <v>27.357142857100001</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.73399559309045903</v>
+        <v>0.73107049608469621</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
@@ -1638,14 +2843,14 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>42.179220000000001</v>
+        <v>42.153846153800004</v>
       </c>
       <c r="B9">
         <v>30</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.71125070591632555</v>
+        <v>0.71167883211756744</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
@@ -1678,14 +2883,14 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>49.879219999999997</v>
+        <v>49.846153846199996</v>
       </c>
       <c r="B10">
         <v>35</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.70169501447697058</v>
+        <v>0.70216049382651036</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
@@ -1718,14 +2923,14 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>45.259219999999999</v>
+        <v>45.2307692308</v>
       </c>
       <c r="B11">
         <v>32</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.70703825651436325</v>
+        <v>0.70748299319679764</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
@@ -1758,14 +2963,14 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>36.019219999999997</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>26</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.72183684155292649</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
@@ -1798,14 +3003,14 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>33.008119999999998</v>
+        <v>33.071428571399998</v>
       </c>
       <c r="B13">
         <v>24</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.72709381812717599</v>
+        <v>0.72570194384511943</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
@@ -1838,14 +3043,14 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>24.368120000000001</v>
+        <v>24.5</v>
       </c>
       <c r="B14">
         <v>18</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.7386700328133643</v>
+        <v>0.73469387755102045</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
@@ -1878,14 +3083,14 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>5.32</v>
+        <v>5.3872053872099999</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.75187969924812026</v>
+        <v>0.74249999999936422</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
@@ -1918,14 +3123,14 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>13.3</v>
+        <v>13.468013468000001</v>
       </c>
       <c r="B16">
         <v>10</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.75187969924812026</v>
+        <v>0.74250000000074245</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
@@ -1958,14 +3163,14 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>34.479219999999998</v>
+        <v>34.5</v>
       </c>
       <c r="B17">
         <v>25</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.72507440713566029</v>
+        <v>0.72463768115942029</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
@@ -1998,14 +3203,14 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>34.479219999999998</v>
+        <v>34.5</v>
       </c>
       <c r="B18">
         <v>25</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.72507440713566029</v>
+        <v>0.72463768115942029</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
@@ -2038,14 +3243,14 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>42.179220000000001</v>
+        <v>42.153846153800004</v>
       </c>
       <c r="B19">
         <v>30</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.71125070591632555</v>
+        <v>0.71167883211756744</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
@@ -2078,14 +3283,14 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>27.24812</v>
+        <v>27.357142857100001</v>
       </c>
       <c r="B20">
         <v>20</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.73399559309045903</v>
+        <v>0.73107049608469621</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
@@ -2118,14 +3323,14 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>13.3</v>
+        <v>13.468013468000001</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0.75187969924812026</v>
+        <v>0.74250000000074245</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
@@ -2158,14 +3363,14 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>6.65</v>
+        <v>6.7340067340100003</v>
       </c>
       <c r="B22">
         <v>5</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>0.75187969924812026</v>
+        <v>0.74249999999963989</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
@@ -2198,14 +3403,14 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>42.179220000000001</v>
+        <v>42.153846153800004</v>
       </c>
       <c r="B23">
         <v>30</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0.71125070591632555</v>
+        <v>0.71167883211756744</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
@@ -2238,14 +3443,14 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>34.479219999999998</v>
+        <v>34.5</v>
       </c>
       <c r="B24">
         <v>25</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>0.72507440713566029</v>
+        <v>0.72463768115942029</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
@@ -2278,14 +3483,14 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>24.368120000000001</v>
+        <v>24.5</v>
       </c>
       <c r="B25">
         <v>18</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>0.7386700328133643</v>
+        <v>0.73469387755102045</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>

</xml_diff>